<commit_message>
Mods Hangar, Avion, Mantenimiento
</commit_message>
<xml_diff>
--- a/Proyecto_final/Insumos/aviones_compania_final.xlsx
+++ b/Proyecto_final/Insumos/aviones_compania_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ovejo\Documents\Universidad-Daniel\Udea\Logica_y_representacion1\Trabajo-Logica---Aerolinea\Proyecto_final\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C4485F-DDA1-4EEF-9180-A433A2972415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10E4A32-9B9E-4511-9335-955394663259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Directorio_Aviones" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Directorio_Aviones!$H$1:$H$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Directorio_Aviones!$B$1:$B$151</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:K151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6612,6 +6612,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B151" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>